<commit_message>
2023 first data delivery! Update SAV
</commit_message>
<xml_diff>
--- a/data-raw/SAV_Table_for_SOE_Report - Laurel Smith - NOAA Federal.xlsx
+++ b/data-raw/SAV_Table_for_SOE_Report - Laurel Smith - NOAA Federal.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laurel.smith\Documents\EDAB\SOE\Habitat\SAVs\2022_SOE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimberly.bastille\Desktop\Rgghhh\ecodata\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12230"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Chart1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Tidal Fresh Total</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>SAV Acres in the Chesapeake Bay by VIMS Bay Salinity Zones. See https://www.chesapeakeprogress.com/abundant-life/sav  and https://www.vims.edu/sav  VIMS 12/10/21</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -2766,23 +2769,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F43" sqref="F42:F43"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2802,7 +2807,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1984</v>
       </c>
@@ -2822,7 +2827,7 @@
         <v>38227.645178999999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1985</v>
       </c>
@@ -2842,7 +2847,7 @@
         <v>49107.898479000003</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1986</v>
       </c>
@@ -2862,7 +2867,7 @@
         <v>47413.662896999995</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1987</v>
       </c>
@@ -2882,7 +2887,7 @@
         <v>49639.95102</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1989</v>
       </c>
@@ -2902,7 +2907,7 @@
         <v>59681.241158999983</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1990</v>
       </c>
@@ -2922,7 +2927,7 @@
         <v>60027.17044799999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1991</v>
       </c>
@@ -2942,7 +2947,7 @@
         <v>63321.863366999998</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1992</v>
       </c>
@@ -2962,7 +2967,7 @@
         <v>70590.20864099999</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1993</v>
       </c>
@@ -2982,7 +2987,7 @@
         <v>73114.190180999984</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1994</v>
       </c>
@@ -3002,7 +3007,7 @@
         <v>65446.119770999998</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1995</v>
       </c>
@@ -3022,7 +3027,7 @@
         <v>59928.598268999995</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1996</v>
       </c>
@@ -3042,7 +3047,7 @@
         <v>63496.372448999988</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1997</v>
       </c>
@@ -3062,7 +3067,7 @@
         <v>69269.232713999983</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1998</v>
       </c>
@@ -3082,7 +3087,7 @@
         <v>63517.500353999989</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1999</v>
       </c>
@@ -3102,7 +3107,7 @@
         <v>68099.697763792006</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2000</v>
       </c>
@@ -3122,7 +3127,7 @@
         <v>69156.476420999999</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2001</v>
       </c>
@@ -3142,7 +3147,7 @@
         <v>85414.475050807538</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2002</v>
       </c>
@@ -3162,7 +3167,7 @@
         <v>89659.069565999991</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2003</v>
       </c>
@@ -3182,7 +3187,7 @@
         <v>63526.929282275458</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2004</v>
       </c>
@@ -3202,7 +3207,7 @@
         <v>72945.315206999992</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2005</v>
       </c>
@@ -3222,7 +3227,7 @@
         <v>78262.900007999997</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2006</v>
       </c>
@@ -3242,7 +3247,7 @@
         <v>59160.432122999999</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2007</v>
       </c>
@@ -3262,7 +3267,7 @@
         <v>64917.477348</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2008</v>
       </c>
@@ -3282,7 +3287,7 @@
         <v>76860.25422599999</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2009</v>
       </c>
@@ -3302,7 +3307,7 @@
         <v>85914.463469999988</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2010</v>
       </c>
@@ -3322,7 +3327,7 @@
         <v>79664.112551999991</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2011</v>
       </c>
@@ -3342,7 +3347,7 @@
         <v>63083.07022947201</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2012</v>
       </c>
@@ -3362,7 +3367,7 @@
         <v>48195.024717</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2013</v>
       </c>
@@ -3382,7 +3387,7 @@
         <v>59711.092321876684</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2014</v>
       </c>
@@ -3402,7 +3407,7 @@
         <v>75438.259730999998</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2015</v>
       </c>
@@ -3422,7 +3427,7 @@
         <v>92314.804271891437</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2016</v>
       </c>
@@ -3442,7 +3447,7 @@
         <v>99618.22066493734</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2017</v>
       </c>
@@ -3462,7 +3467,7 @@
         <v>104892.87621719918</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2018</v>
       </c>
@@ -3482,7 +3487,7 @@
         <v>108077.86083382118</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2019</v>
       </c>
@@ -3502,7 +3507,7 @@
         <v>66684.118055899802</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2020</v>
       </c>
@@ -3522,12 +3527,25 @@
         <v>63131.589072218638</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2021</v>
+      </c>
+      <c r="B39" s="1">
+        <v>19173</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="1">
+        <v>16132</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>